<commit_message>
uptdate mapa de procesos v2
</commit_message>
<xml_diff>
--- a/01_Documentacion/12_Diagrama de proceso/IR_MAPA_PROC_10N_V2.xlsx
+++ b/01_Documentacion/12_Diagrama de proceso/IR_MAPA_PROC_10N_V2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\ING_REQUISITOS\GITHUB\EspinAndres_14568_G2_IR\01_Documentacion\12_Diagrama de proceso\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7332EF34-95F1-448D-B7A7-A2151403B9F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{438177BC-D538-49E9-ACBB-AA4C72170BFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4997B183-6BA5-427C-8615-A6F9FCD80629}"/>
   </bookViews>
@@ -826,7 +826,7 @@
               <a:ea typeface="+mn-lt"/>
               <a:cs typeface="+mn-lt"/>
             </a:rPr>
-            <a:t>Planificar envío del Vendedor al Territorio Rural</a:t>
+            <a:t>1. Planificar envío del Vendedor al Territorio Rural</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -905,7 +905,7 @@
               </a:solidFill>
               <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>Designar</a:t>
+            <a:t>2. Designar</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
@@ -991,7 +991,7 @@
               <a:ea typeface="+mn-lt"/>
               <a:cs typeface="+mn-lt"/>
             </a:rPr>
-            <a:t>Recolectar información de Interesados Potenciales</a:t>
+            <a:t>4.Recolectar información de Interesados Potenciales</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1052,7 +1052,7 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="en-US"/>
-            <a:t>Realizar la reunión con el Representante del Territorio Rural</a:t>
+            <a:t>5. Realizar la reunión con el Representante del Territorio Rural</a:t>
           </a:r>
           <a:endParaRPr lang="es-EC" sz="1100"/>
         </a:p>
@@ -1124,7 +1124,7 @@
               <a:ea typeface="+mn-lt"/>
               <a:cs typeface="+mn-lt"/>
             </a:rPr>
-            <a:t>Elaborar del Contrato Preliminar</a:t>
+            <a:t>6. Elaborar del Contrato Preliminar</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1195,7 +1195,7 @@
               <a:ea typeface="+mn-lt"/>
               <a:cs typeface="+mn-lt"/>
             </a:rPr>
-            <a:t>Revisar el Contrato y Documentación</a:t>
+            <a:t>7. Revisar el Contrato y Documentación</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1266,7 +1266,7 @@
               <a:ea typeface="+mn-lt"/>
               <a:cs typeface="+mn-lt"/>
             </a:rPr>
-            <a:t>Contratar Freelancers para Ayuda en la Instalación</a:t>
+            <a:t>8. Contratar Freelancers para Ayuda en la Instalación</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1330,7 +1330,7 @@
           <a:pPr marL="0" indent="0" algn="l"/>
           <a:r>
             <a:rPr lang="en-US"/>
-            <a:t>Ejecutar la Instalación</a:t>
+            <a:t>9. Ejecutar la Instalación</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
             <a:solidFill>
@@ -5210,7 +5210,7 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="en-US"/>
-            <a:t>Promocionar los planes de internet en la Localidad Rural</a:t>
+            <a:t>3. Promocionar los planes de internet en la Localidad Rural</a:t>
           </a:r>
           <a:endParaRPr lang="es-EC" sz="1100"/>
         </a:p>
@@ -5601,7 +5601,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>463074</xdr:colOff>
+      <xdr:colOff>584790</xdr:colOff>
       <xdr:row>53</xdr:row>
       <xdr:rowOff>106265</xdr:rowOff>
     </xdr:to>
@@ -5618,8 +5618,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8531700" y="8475985"/>
-          <a:ext cx="1363898" cy="387731"/>
+          <a:off x="8557077" y="9658513"/>
+          <a:ext cx="1490690" cy="1363845"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5646,7 +5646,11 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="en-US"/>
-            <a:t>Registrar a las personas interesadas en contratar los planes de internet.</a:t>
+            <a:t>Registrar a las personas interesadas en contratar los planes de internet, se registra cédula, acta</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" baseline="0"/>
+            <a:t> de acuerdo firmada y dirección de domicilio.</a:t>
           </a:r>
           <a:endParaRPr lang="es-EC" sz="1100"/>
         </a:p>
@@ -8639,93 +8643,6 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>112644</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>185531</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>417443</xdr:colOff>
-      <xdr:row>80</xdr:row>
-      <xdr:rowOff>53009</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="TextBox 11">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5080CFDB-102E-BEDF-FD49-5778BAB00914}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6473687" y="14067183"/>
-          <a:ext cx="2690191" cy="1981200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Del tema sistema, la</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> dueña puede mandar mensajes dentro de este medio y los trabajadores pueden acceder a estas notificaciones. </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>Hoja de ruta, cuando recién se va a entrar a la comunidad. </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>Modelo de aplicación, reglamento o normativa interna de la empresa, algo asi como estatutos. También en el ámbito de seguridad,  debe existir. </a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -9048,8 +8965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CAE3A4D-6C57-42F5-813D-06E56D78CC84}">
   <dimension ref="A2:BA92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="86" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K124" sqref="K124"/>
+    <sheetView tabSelected="1" topLeftCell="C14" zoomScale="86" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9816,6 +9733,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="f1f31ffb-9912-4459-99c8-b26e82094b51" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100EDB39E34F5A9B445B025C05B2A05D030" ma:contentTypeVersion="9" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="f14866ee3587f7ce27492aa7a9fad3cb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f1f31ffb-9912-4459-99c8-b26e82094b51" xmlns:ns4="ce621958-37b1-43fe-a1f1-1aad67996a88" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4a75488916cf2c0345e17416545d11eb" ns3:_="" ns4:_="">
     <xsd:import namespace="f1f31ffb-9912-4459-99c8-b26e82094b51"/>
@@ -10010,24 +9944,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A51AD67E-59C2-4671-B80A-68814504A7B3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="f1f31ffb-9912-4459-99c8-b26e82094b51"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="ce621958-37b1-43fe-a1f1-1aad67996a88"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="f1f31ffb-9912-4459-99c8-b26e82094b51" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D2E9C9A-9A36-40CB-B367-1FF07A2FA447}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00F2870E-899D-461B-8DB6-B19C05AA0D61}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10044,29 +9986,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D2E9C9A-9A36-40CB-B367-1FF07A2FA447}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A51AD67E-59C2-4671-B80A-68814504A7B3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="f1f31ffb-9912-4459-99c8-b26e82094b51"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="ce621958-37b1-43fe-a1f1-1aad67996a88"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update diagrama de procesos
</commit_message>
<xml_diff>
--- a/01_Documentacion/12_Diagrama de proceso/IR_MAPA_PROC_10N_V2.xlsx
+++ b/01_Documentacion/12_Diagrama de proceso/IR_MAPA_PROC_10N_V2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\ING_REQUISITOS\GITHUB\EspinAndres_14568_G2_IR\01_Documentacion\12_Diagrama de proceso\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{438177BC-D538-49E9-ACBB-AA4C72170BFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24DB49C7-40DD-4A6F-AF45-D5762D4030D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4997B183-6BA5-427C-8615-A6F9FCD80629}"/>
   </bookViews>
@@ -826,7 +826,29 @@
               <a:ea typeface="+mn-lt"/>
               <a:cs typeface="+mn-lt"/>
             </a:rPr>
-            <a:t>1. Planificar envío del Vendedor al Territorio Rural</a:t>
+            <a:t>1. Planificar envío de</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-lt"/>
+              <a:cs typeface="+mn-lt"/>
+            </a:rPr>
+            <a:t> la Secretaria</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-lt"/>
+              <a:cs typeface="+mn-lt"/>
+            </a:rPr>
+            <a:t> al Territorio Rural</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -8965,8 +8987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CAE3A4D-6C57-42F5-813D-06E56D78CC84}">
   <dimension ref="A2:BA92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C14" zoomScale="86" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="Q19" sqref="Q19"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="86" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9733,23 +9755,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="f1f31ffb-9912-4459-99c8-b26e82094b51" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100EDB39E34F5A9B445B025C05B2A05D030" ma:contentTypeVersion="9" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="f14866ee3587f7ce27492aa7a9fad3cb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f1f31ffb-9912-4459-99c8-b26e82094b51" xmlns:ns4="ce621958-37b1-43fe-a1f1-1aad67996a88" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4a75488916cf2c0345e17416545d11eb" ns3:_="" ns4:_="">
     <xsd:import namespace="f1f31ffb-9912-4459-99c8-b26e82094b51"/>
@@ -9944,32 +9949,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A51AD67E-59C2-4671-B80A-68814504A7B3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="f1f31ffb-9912-4459-99c8-b26e82094b51"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="ce621958-37b1-43fe-a1f1-1aad67996a88"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D2E9C9A-9A36-40CB-B367-1FF07A2FA447}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="f1f31ffb-9912-4459-99c8-b26e82094b51" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00F2870E-899D-461B-8DB6-B19C05AA0D61}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9986,4 +9983,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D2E9C9A-9A36-40CB-B367-1FF07A2FA447}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A51AD67E-59C2-4671-B80A-68814504A7B3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="f1f31ffb-9912-4459-99c8-b26e82094b51"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="ce621958-37b1-43fe-a1f1-1aad67996a88"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>